<commit_message>
multiple test cases added with enhancement
1. added test image
2. Template Analytics and Reporting
3. improved template metadata
4. added path walk
5. flow improvements with minor bug fixes, xpath modify and proper delay
6. commonUtils function - Stale element retry logic
7. api reqSpec function modify for form data API
</commit_message>
<xml_diff>
--- a/Data_Files/Demo_3_Data_433_BulkUpload.xlsx
+++ b/Data_Files/Demo_3_Data_433_BulkUpload.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soumya\Documents\GitHub\Git 1Channel Portal UI\Assistive-Portal-UI-Automation-Preprod\Data_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soumya\Documents\GitHub\1Channel-E2E_TestAutomation-Preprod\1Channel-E2E_TestAutomation-Preprod\Data_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0C3A4C-3085-435E-B56F-3B8F459D4D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9765D0D-91CE-4300-98D5-B37652D0E240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="81">
   <si>
     <t>FGM</t>
   </si>
@@ -262,6 +262,12 @@
   </si>
   <si>
     <t>Cust 10A 333</t>
+  </si>
+  <si>
+    <t>Branch email ID</t>
+  </si>
+  <si>
+    <t>be1@ig.com</t>
   </si>
 </sst>
 </file>
@@ -311,24 +317,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -610,751 +609,820 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BI4"/>
+  <dimension ref="A1:BJ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AQ7" sqref="AQ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="26.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="31.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="23.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="28.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="6.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="7.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="13.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="12.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="25.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="25.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="27.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="16.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="15.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="25.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="63" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="2" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:62" s="1" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:61" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="4">
         <v>91102001</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="4">
         <v>91223344</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="4">
         <v>8102020003</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="L2" s="3" t="s">
+      <c r="J2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>66</v>
       </c>
       <c r="M2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="R2" s="3">
+      <c r="O2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="S2" s="4">
         <v>200</v>
       </c>
-      <c r="S2" s="3">
+      <c r="T2" s="4">
         <v>502</v>
       </c>
-      <c r="T2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="U2">
+      <c r="U2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="V2" s="4">
         <v>100</v>
       </c>
-      <c r="V2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI2" t="s">
+      <c r="W2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AJ2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AL2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AK2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AQ2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS2" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AS2" s="3" t="s">
+      <c r="AT2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AU2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AU2" s="5" t="s">
+      <c r="AV2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="AV2" s="6"/>
-      <c r="AW2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AX2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AY2" s="3" t="s">
+      <c r="AW2" s="3"/>
+      <c r="AX2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AY2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AZ2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="AZ2" s="3" t="s">
+      <c r="BA2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="BA2" s="3"/>
-      <c r="BB2" s="3" t="s">
+      <c r="BC2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="BC2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="BD2" s="3" t="s">
+      <c r="BD2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="BE2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="BE2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="BF2" s="3" t="s">
+      <c r="BF2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="BG2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="BG2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="BH2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="BI2" s="3" t="s">
+      <c r="BH2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="BI2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="BJ2" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:61" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="4">
         <v>91102002</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="4">
         <v>91223345</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="4">
         <v>8102020010</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="L3" s="3" t="s">
+      <c r="J3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>66</v>
       </c>
       <c r="M3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="R3" s="3">
+      <c r="O3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="S3" s="4">
         <v>100</v>
       </c>
-      <c r="S3" s="3">
+      <c r="T3" s="4">
         <v>509</v>
       </c>
-      <c r="T3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="U3">
+      <c r="U3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="V3" s="4">
         <v>50</v>
       </c>
-      <c r="V3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AG3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI3" t="s">
+      <c r="W3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ3" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AJ3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AL3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AM3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AN3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AO3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AP3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AQ3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AR3" s="3" t="s">
+      <c r="AK3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AN3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AQ3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS3" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="AS3" s="3" t="s">
+      <c r="AT3" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AT3" s="3" t="s">
+      <c r="AU3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AU3" s="5" t="s">
+      <c r="AV3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="AV3" s="6"/>
-      <c r="AW3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AX3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AY3" s="3" t="s">
+      <c r="AW3" s="3"/>
+      <c r="AX3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AY3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AZ3" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="AZ3" s="3" t="s">
+      <c r="BA3" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="BA3" s="3"/>
-      <c r="BB3" s="3" t="s">
+      <c r="BC3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="BC3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="BD3" s="3" t="s">
+      <c r="BD3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="BE3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="BE3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="BF3" s="3" t="s">
+      <c r="BF3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="BG3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="BG3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="BH3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="BI3" s="3" t="s">
+      <c r="BH3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="BI3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="BJ3" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:61" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="4">
         <v>91102003</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="4">
         <v>91223346</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="4">
         <v>8102020013</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="L4" s="3" t="s">
+      <c r="J4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>66</v>
       </c>
       <c r="M4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N4" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="N4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="R4" s="3">
+      <c r="O4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="S4" s="4">
         <v>110</v>
       </c>
-      <c r="S4" s="3">
+      <c r="T4" s="4">
         <v>512</v>
       </c>
-      <c r="T4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="U4">
+      <c r="U4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="V4" s="4">
         <v>75</v>
       </c>
-      <c r="V4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI4" t="s">
+      <c r="W4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ4" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AJ4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AL4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AM4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AN4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AP4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AQ4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AR4" s="3" t="s">
+      <c r="AK4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AN4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AQ4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS4" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="AS4" s="3" t="s">
+      <c r="AT4" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AT4" s="3" t="s">
+      <c r="AU4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AU4" s="5" t="s">
+      <c r="AV4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="AV4" s="6"/>
-      <c r="AW4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AX4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AY4" s="3" t="s">
+      <c r="AW4" s="3"/>
+      <c r="AX4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AY4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AZ4" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="AZ4" s="3" t="s">
+      <c r="BA4" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="BA4" s="3"/>
-      <c r="BB4" s="3" t="s">
+      <c r="BC4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="BC4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="BD4" s="3" t="s">
+      <c r="BD4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="BE4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="BE4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="BF4" s="3" t="s">
+      <c r="BF4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="BG4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="BG4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="BH4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="BI4" s="3" t="s">
+      <c r="BH4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="BI4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="BJ4" s="4" t="s">
         <v>72</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AU2" r:id="rId1" xr:uid="{745DED01-742A-4573-BD0D-91DC9B3DF1F8}"/>
-    <hyperlink ref="AU3:AU4" r:id="rId2" display="inbsom@gmail.com" xr:uid="{65C93AA3-874D-4D60-AF50-EC8F568CEE30}"/>
+    <hyperlink ref="AV2" r:id="rId1" xr:uid="{745DED01-742A-4573-BD0D-91DC9B3DF1F8}"/>
+    <hyperlink ref="AV3:AV4" r:id="rId2" display="inbsom@gmail.com" xr:uid="{65C93AA3-874D-4D60-AF50-EC8F568CEE30}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{7E8B8194-7058-4575-912F-7A838B5E6EEF}"/>
+    <hyperlink ref="E3:E4" r:id="rId4" display="be1@ig.com" xr:uid="{BA63DDFB-2F0C-46CF-B709-726BA890FE89}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
debug_matches implement & minor enhancement
1. implemented debug matches functionality
2. enhanced bulk upload customer for 433 with parameterized test accounts
</commit_message>
<xml_diff>
--- a/Data_Files/Demo_3_Data_433_BulkUpload.xlsx
+++ b/Data_Files/Demo_3_Data_433_BulkUpload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soumya\Documents\GitHub\1Channel-E2E_TestAutomation-Preprod\1Channel-E2E_TestAutomation-Preprod\Data_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9765D0D-91CE-4300-98D5-B37652D0E240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0497802-97EF-43DA-8DB7-7251F513FFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="83">
   <si>
     <t>FGM</t>
   </si>
@@ -210,9 +210,6 @@
     <t>Promised to Pay Break - Visit</t>
   </si>
   <si>
-    <t>KOLKATA</t>
-  </si>
-  <si>
     <t>KOLKATA NORTH</t>
   </si>
   <si>
@@ -268,13 +265,22 @@
   </si>
   <si>
     <t>be1@ig.com</t>
+  </si>
+  <si>
+    <t>KOL_01</t>
+  </si>
+  <si>
+    <t>KOL_02</t>
+  </si>
+  <si>
+    <t>KOL_03</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,6 +297,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -317,7 +329,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -326,8 +338,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -611,73 +622,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AQ7" sqref="AQ7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="26.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="31.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="23.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="28.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="6.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="7.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="15.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="13.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="12.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="25.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="13.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="25.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="27.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="16.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="15.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="25.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="63" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="25.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:62" s="1" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -694,7 +704,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -869,555 +879,556 @@
       </c>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" s="4">
+      <c r="G2">
         <v>91102001</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2">
         <v>91223344</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2">
         <v>8102020003</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" t="s">
+        <v>65</v>
+      </c>
+      <c r="P2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>65</v>
+      </c>
+      <c r="R2" t="s">
+        <v>65</v>
+      </c>
+      <c r="S2">
+        <v>200</v>
+      </c>
+      <c r="T2">
+        <v>502</v>
+      </c>
+      <c r="U2" t="s">
+        <v>65</v>
+      </c>
+      <c r="V2">
+        <v>100</v>
+      </c>
+      <c r="W2" t="s">
+        <v>65</v>
+      </c>
+      <c r="X2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT2" t="s">
         <v>67</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="S2" s="4">
-        <v>200</v>
-      </c>
-      <c r="T2" s="4">
-        <v>502</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="V2" s="4">
-        <v>100</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AG2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ2" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AK2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AL2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AM2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AN2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AO2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AP2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AQ2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AR2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS2" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="AT2" s="4" t="s">
+      <c r="AU2" t="s">
         <v>68</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AV2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AW2" s="3"/>
+      <c r="AX2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AZ2" t="s">
         <v>69</v>
       </c>
-      <c r="AV2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AW2" s="3"/>
-      <c r="AX2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AY2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AZ2" s="4" t="s">
+      <c r="BA2" t="s">
         <v>70</v>
       </c>
-      <c r="BA2" s="4" t="s">
+      <c r="BC2" t="s">
         <v>71</v>
       </c>
-      <c r="BC2" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="BD2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="BE2" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="BF2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="BG2" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="BH2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="BI2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="BJ2" s="4" t="s">
-        <v>72</v>
+      <c r="BD2" t="s">
+        <v>65</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>71</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>65</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>71</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>65</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>65</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" s="4">
+      <c r="G3">
         <v>91102002</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3">
         <v>91223345</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3">
         <v>8102020010</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" t="s">
+        <v>65</v>
+      </c>
+      <c r="L3" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="N3" s="5" t="s">
+      <c r="O3" t="s">
+        <v>65</v>
+      </c>
+      <c r="P3" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>65</v>
+      </c>
+      <c r="R3" t="s">
+        <v>65</v>
+      </c>
+      <c r="S3">
+        <v>100</v>
+      </c>
+      <c r="T3">
+        <v>509</v>
+      </c>
+      <c r="U3" t="s">
+        <v>65</v>
+      </c>
+      <c r="V3">
+        <v>50</v>
+      </c>
+      <c r="W3" t="s">
+        <v>65</v>
+      </c>
+      <c r="X3" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT3" t="s">
         <v>67</v>
       </c>
-      <c r="O3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="S3" s="4">
-        <v>100</v>
-      </c>
-      <c r="T3" s="4">
-        <v>509</v>
-      </c>
-      <c r="U3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="V3" s="4">
-        <v>50</v>
-      </c>
-      <c r="W3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="X3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AG3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ3" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AK3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AL3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AM3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AN3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AO3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AP3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AQ3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AR3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS3" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AT3" s="4" t="s">
+      <c r="AU3" t="s">
         <v>68</v>
       </c>
-      <c r="AU3" s="4" t="s">
+      <c r="AV3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AW3" s="3"/>
+      <c r="AX3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AZ3" t="s">
         <v>69</v>
       </c>
-      <c r="AV3" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AW3" s="3"/>
-      <c r="AX3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AY3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AZ3" s="4" t="s">
+      <c r="BA3" t="s">
         <v>70</v>
       </c>
-      <c r="BA3" s="4" t="s">
+      <c r="BC3" t="s">
         <v>71</v>
       </c>
-      <c r="BC3" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="BD3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="BE3" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="BF3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="BG3" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="BH3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="BI3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="BJ3" s="4" t="s">
-        <v>72</v>
+      <c r="BD3" t="s">
+        <v>65</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>71</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>65</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>71</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>65</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>65</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4">
+        <v>91102003</v>
+      </c>
+      <c r="H4">
+        <v>91223346</v>
+      </c>
+      <c r="I4">
+        <v>8102020013</v>
+      </c>
+      <c r="J4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M4" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="O4" t="s">
+        <v>65</v>
+      </c>
+      <c r="P4" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>65</v>
+      </c>
+      <c r="R4" t="s">
+        <v>65</v>
+      </c>
+      <c r="S4">
+        <v>110</v>
+      </c>
+      <c r="T4">
+        <v>512</v>
+      </c>
+      <c r="U4" t="s">
+        <v>65</v>
+      </c>
+      <c r="V4">
+        <v>75</v>
+      </c>
+      <c r="W4" t="s">
+        <v>65</v>
+      </c>
+      <c r="X4" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AV4" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G4" s="4">
-        <v>91102003</v>
-      </c>
-      <c r="H4" s="4">
-        <v>91223346</v>
-      </c>
-      <c r="I4" s="4">
-        <v>8102020013</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="S4" s="4">
-        <v>110</v>
-      </c>
-      <c r="T4" s="4">
-        <v>512</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="V4" s="4">
-        <v>75</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="X4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AG4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ4" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AK4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AL4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AM4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AN4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AO4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AP4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AQ4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AR4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS4" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="AT4" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AU4" s="4" t="s">
+      <c r="AW4" s="3"/>
+      <c r="AX4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AZ4" t="s">
         <v>69</v>
       </c>
-      <c r="AV4" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AW4" s="3"/>
-      <c r="AX4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AY4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AZ4" s="4" t="s">
+      <c r="BA4" t="s">
         <v>70</v>
       </c>
-      <c r="BA4" s="4" t="s">
+      <c r="BC4" t="s">
         <v>71</v>
       </c>
-      <c r="BC4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="BD4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="BE4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="BF4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="BG4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="BH4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="BI4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="BJ4" s="4" t="s">
-        <v>72</v>
+      <c r="BD4" t="s">
+        <v>65</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>71</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>65</v>
+      </c>
+      <c r="BG4" t="s">
+        <v>71</v>
+      </c>
+      <c r="BH4" t="s">
+        <v>65</v>
+      </c>
+      <c r="BI4" t="s">
+        <v>65</v>
+      </c>
+      <c r="BJ4" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="AV2" r:id="rId1" xr:uid="{745DED01-742A-4573-BD0D-91DC9B3DF1F8}"/>
     <hyperlink ref="AV3:AV4" r:id="rId2" display="inbsom@gmail.com" xr:uid="{65C93AA3-874D-4D60-AF50-EC8F568CEE30}"/>

</xml_diff>